<commit_message>
mallet & package list
</commit_message>
<xml_diff>
--- a/mypackages.xlsx
+++ b/mypackages.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvera\Documents\Code\h-r\miscelanea\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tidyviz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="201">
   <si>
     <t>Amelia</t>
   </si>
@@ -624,6 +624,9 @@
   </si>
   <si>
     <t>Boruta</t>
+  </si>
+  <si>
+    <t>mallet</t>
   </si>
 </sst>
 </file>
@@ -975,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A201"/>
+  <dimension ref="A1:A202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,491 +1508,496 @@
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>59</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>198</v>
+        <v>61</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>143</v>
+        <v>198</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>144</v>
+        <v>62</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>183</v>
+        <v>63</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>146</v>
+        <v>64</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>65</v>
+        <v>147</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>149</v>
+        <v>72</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>153</v>
+        <v>74</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>155</v>
+        <v>75</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>156</v>
+        <v>76</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>77</v>
+        <v>158</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>159</v>
+        <v>80</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>81</v>
+        <v>161</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>83</v>
+        <v>164</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>193</v>
+        <v>89</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>189</v>
+        <v>93</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>94</v>
+        <v>174</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>173</v>
+        <v>95</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>96</v>
+        <v>173</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>175</v>
+        <v>97</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>98</v>
+        <v>175</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>176</v>
+        <v>98</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>99</v>
+        <v>176</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>186</v>
+        <v>100</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>101</v>
+        <v>186</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>194</v>
+        <v>102</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>177</v>
+        <v>103</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A201">
+  <sortState ref="A2:A202">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>